<commit_message>
Change comments in TemplateExcelFileGenerator
</commit_message>
<xml_diff>
--- a/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImages_Channel1.xlsx
+++ b/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImages_Channel1.xlsx
@@ -12,9 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Put the path to images of the channel in this file</t>
+    <t>Put the path to images under the corresponding title.</t>
+  </si>
+  <si>
+    <t>The files in each row must correspond to different polarizations of same sample.</t>
   </si>
   <si>
     <t>The path must be the remaining path after the root folder, which is:</t>
@@ -68,7 +71,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -107,16 +110,27 @@
       <c r="E3"/>
       <c r="F3"/>
     </row>
-    <row r="5">
-      <c r="A5" t="s">
+    <row r="4">
+      <c r="A4" t="s">
         <v>3</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:F1"/>
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A3:F3"/>
+    <mergeCell ref="A4:F4"/>
   </mergeCells>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Remove condition in isFile in createChannelFile
</commit_message>
<xml_diff>
--- a/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImages_Channel1.xlsx
+++ b/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel/SampleImages_Channel1.xlsx
@@ -14,16 +14,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
-    <t>Put the path to images under the corresponding title.</t>
-  </si>
-  <si>
-    <t>The files in each row must correspond to different polarizations of same sample.</t>
+    <t>Put the path to the images under the corresponding column.</t>
   </si>
   <si>
     <t>The path must be the remaining path after the root folder, which is:</t>
   </si>
   <si>
     <t>/home/masoud/Documents/four-polar/fourPolar-io/target/test-classes/fr/fresnel/fourPolar/io/imageSet/acquisition/sample/finders/excel</t>
+  </si>
+  <si>
+    <t>The files in each row must correspond to different polarizations of same sample.</t>
   </si>
   <si>
     <t>Pol0_45_90_135</t>

</xml_diff>